<commit_message>
Save and load today achievements done frmTodoList
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Start at</t>
+  </si>
+  <si>
+    <t>4:20 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Today </t>
+  </si>
+  <si>
+    <t>Target(s)</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>09/26/2019</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Targets</t>
+  </si>
   <si>
     <t>Point</t>
   </si>
@@ -30,7 +57,13 @@
     <t>DateTime</t>
   </si>
   <si>
+    <t>Achievement</t>
+  </si>
+  <si>
     <t>Total points</t>
+  </si>
+  <si>
+    <t>Total working day</t>
   </si>
   <si>
     <t>Relax day</t>
@@ -42,23 +75,28 @@
     <t>Challenge</t>
   </si>
   <si>
-    <t>Total working day</t>
+    <t>Total lucky</t>
   </si>
   <si>
-    <t>Targets</t>
-  </si>
-  <si>
-    <t>Attendance</t>
+    <t>Total incomplete targets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,16 +122,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="18" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+      <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -375,70 +420,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DXD13"/>
+  <dimension ref="A1:DXD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="2" customWidth="1"/>
-    <col min="4" max="7" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" bestFit="1" width="23" customWidth="1" style="2"/>
+    <col min="2" max="2" width="20" customWidth="1" style="2"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1" style="2"/>
+    <col min="4" max="8" bestFit="1" width="9.7109375" customWidth="1" style="2"/>
+    <col min="9" max="10" bestFit="1" width="10.7109375" customWidth="1" style="2"/>
+    <col min="11" max="26" width="9.140625" customWidth="1" style="2"/>
+    <col min="27" max="16384" width="9.140625" customWidth="1" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3332" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3332" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B3" s="2">
         <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3332" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -3768,76 +3786,158 @@
       <c r="DXC3" s="3"/>
       <c r="DXD3" s="3"/>
     </row>
-    <row r="4" spans="1:3332" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3">
         <v>43731</v>
       </c>
-      <c r="C4" s="3">
-        <v>43732</v>
+      <c r="C11" s="3">
+        <v>43735</v>
       </c>
-      <c r="D4" s="3">
-        <v>43733</v>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
       </c>
-      <c r="E4" s="3">
-        <v>43734</v>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3332" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="B13" s="2">
         <v>103</v>
       </c>
+      <c r="G13" s="1"/>
     </row>
-    <row r="7" spans="1:3332" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B14" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:3332" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>15</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B15" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:3332" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B16" s="2">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3332" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>17</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B17" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3332" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>18</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B18" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:3332" x14ac:dyDescent="0.25">
-      <c r="G13" s="1"/>
+    <row r="19">
+      <c r="A19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A12:B12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create updateAchievement and change some variable name
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -24,7 +24,7 @@
     <t>Start at</t>
   </si>
   <si>
-    <t>4:20 PM</t>
+    <t>5:20 PM</t>
   </si>
   <si>
     <t xml:space="preserve">Today </t>
@@ -423,7 +423,7 @@
   <dimension ref="A1:DXD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,8 +433,8 @@
     <col min="3" max="3" width="11.42578125" customWidth="1" style="2"/>
     <col min="4" max="8" bestFit="1" width="9.7109375" customWidth="1" style="2"/>
     <col min="9" max="10" bestFit="1" width="10.7109375" customWidth="1" style="2"/>
-    <col min="11" max="26" width="9.140625" customWidth="1" style="2"/>
-    <col min="27" max="16384" width="9.140625" customWidth="1" style="2"/>
+    <col min="11" max="31" width="9.140625" customWidth="1" style="2"/>
+    <col min="32" max="16384" width="9.140625" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -456,7 +456,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -3791,7 +3791,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -3799,7 +3799,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -3820,45 +3820,23 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3">
-        <v>43731</v>
-      </c>
-      <c r="C11" s="3">
-        <v>43735</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -3878,7 +3856,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -3887,7 +3865,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -3895,7 +3873,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -3903,7 +3881,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -3911,7 +3889,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -3919,7 +3897,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -3927,7 +3905,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove unnecessary events in frmTodoList
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -19,12 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Start at</t>
   </si>
   <si>
-    <t>5:20 PM</t>
+    <t>9:44 AM</t>
   </si>
   <si>
     <t xml:space="preserve">Today </t>
@@ -39,7 +39,7 @@
     <t>Incomplete</t>
   </si>
   <si>
-    <t>09/26/2019</t>
+    <t>09/27/2019</t>
   </si>
   <si>
     <t>History</t>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>DateTime</t>
+  </si>
+  <si>
+    <t>09/26/2019</t>
   </si>
   <si>
     <t>Achievement</t>
@@ -456,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -3799,7 +3802,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -3820,22 +3823,33 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -3847,30 +3861,30 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -3878,7 +3892,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -3886,7 +3900,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -3894,7 +3908,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -3902,10 +3916,10 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add save luckypoint and load luckypoint
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -19,12 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Start at</t>
   </si>
   <si>
     <t>9:44 AM</t>
+  </si>
+  <si>
+    <t>Lucky</t>
+  </si>
+  <si>
+    <t>True</t>
   </si>
   <si>
     <t xml:space="preserve">Today </t>
@@ -426,7 +432,7 @@
   <dimension ref="A1:DXD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,8 +442,8 @@
     <col min="3" max="3" width="11.42578125" customWidth="1" style="2"/>
     <col min="4" max="8" bestFit="1" width="9.7109375" customWidth="1" style="2"/>
     <col min="9" max="10" bestFit="1" width="10.7109375" customWidth="1" style="2"/>
-    <col min="11" max="31" width="9.140625" customWidth="1" style="2"/>
-    <col min="32" max="16384" width="9.140625" customWidth="1" style="2"/>
+    <col min="11" max="33" width="9.140625" customWidth="1" style="2"/>
+    <col min="34" max="16384" width="9.140625" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -447,16 +453,25 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -3791,7 +3806,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -3799,7 +3814,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -3807,21 +3822,21 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="6"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <v>3</v>
@@ -3829,7 +3844,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -3837,7 +3852,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
@@ -3845,10 +3860,10 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -3861,13 +3876,13 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
@@ -3876,7 +3891,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2">
         <v>1</v>
@@ -3884,7 +3899,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -3892,7 +3907,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -3900,7 +3915,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -3908,7 +3923,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -3916,7 +3931,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
delete some unnecessary files part 2
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -19,12 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Start at</t>
   </si>
   <si>
-    <t>9:44 AM</t>
+    <t>10:14 AM</t>
   </si>
   <si>
     <t>Lucky</t>
@@ -45,7 +45,7 @@
     <t>Incomplete</t>
   </si>
   <si>
-    <t>09/27/2019</t>
+    <t>10/01/2019</t>
   </si>
   <si>
     <t>History</t>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>09/26/2019</t>
+  </si>
+  <si>
+    <t>09/27/2019</t>
   </si>
   <si>
     <t>Achievement</t>
@@ -432,7 +435,7 @@
   <dimension ref="A1:DXD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,8 +445,8 @@
     <col min="3" max="3" width="11.42578125" customWidth="1" style="2"/>
     <col min="4" max="8" bestFit="1" width="9.7109375" customWidth="1" style="2"/>
     <col min="9" max="10" bestFit="1" width="10.7109375" customWidth="1" style="2"/>
-    <col min="11" max="33" width="9.140625" customWidth="1" style="2"/>
-    <col min="34" max="16384" width="9.140625" customWidth="1" style="2"/>
+    <col min="11" max="34" width="9.140625" customWidth="1" style="2"/>
+    <col min="35" max="16384" width="9.140625" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3841,6 +3844,9 @@
       <c r="B8" s="2">
         <v>3</v>
       </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -3849,6 +3855,9 @@
       <c r="B9" s="2">
         <v>1</v>
       </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -3857,6 +3866,9 @@
       <c r="B10" s="2">
         <v>2</v>
       </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -3865,7 +3877,9 @@
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -3876,30 +3890,30 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -3907,15 +3921,15 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -3923,15 +3937,15 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Add ResetLuckyStatus and ClearTodayHistory
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,12 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Start at</t>
   </si>
   <si>
-    <t>10:14 AM</t>
+    <t>10:35 AM</t>
   </si>
   <si>
     <t>Lucky</t>
@@ -97,8 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,21 +134,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
-    <xf numFmtId="18" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -435,21 +434,21 @@
   <dimension ref="A1:DXD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="23" customWidth="1" style="2"/>
-    <col min="2" max="2" width="20" customWidth="1" style="2"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1" style="2"/>
-    <col min="4" max="8" bestFit="1" width="9.7109375" customWidth="1" style="2"/>
-    <col min="9" max="10" bestFit="1" width="10.7109375" customWidth="1" style="2"/>
-    <col min="11" max="34" width="9.140625" customWidth="1" style="2"/>
-    <col min="35" max="16384" width="9.140625" customWidth="1" style="2"/>
+    <col min="1" max="1" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2" customWidth="1"/>
+    <col min="4" max="8" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="39" width="9.140625" style="2" customWidth="1"/>
+    <col min="40" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -463,16 +462,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="2">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -3807,7 +3806,7 @@
       <c r="DXC3" s="3"/>
       <c r="DXD3" s="3"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -3815,7 +3814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -3823,7 +3822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -3831,13 +3830,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -3848,7 +3847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -3859,7 +3858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -3870,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -3888,46 +3887,46 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3332" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3935,15 +3934,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="2">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -3952,13 +3951,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="3">
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add close frmTodoList when open frmDetails
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Start at</t>
   </si>
@@ -97,7 +97,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,21 +135,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="18" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -434,21 +435,21 @@
   <dimension ref="A1:DXD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="2" customWidth="1"/>
-    <col min="4" max="8" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="39" width="9.140625" style="2" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" bestFit="1" width="23" customWidth="1" style="2"/>
+    <col min="2" max="2" width="20" customWidth="1" style="2"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1" style="2"/>
+    <col min="4" max="8" bestFit="1" width="9.7109375" customWidth="1" style="2"/>
+    <col min="9" max="10" bestFit="1" width="10.7109375" customWidth="1" style="2"/>
+    <col min="11" max="40" width="9.140625" customWidth="1" style="2"/>
+    <col min="41" max="16384" width="9.140625" customWidth="1" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -465,13 +466,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -3806,7 +3807,7 @@
       <c r="DXC3" s="3"/>
       <c r="DXD3" s="3"/>
     </row>
-    <row r="4" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -3814,7 +3815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -3822,7 +3823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -3830,13 +3831,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -3846,8 +3847,11 @@
       <c r="C8" s="2">
         <v>1</v>
       </c>
+      <c r="D8" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -3857,8 +3861,11 @@
       <c r="C9" s="2">
         <v>1</v>
       </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="10" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -3868,8 +3875,11 @@
       <c r="C10" s="2">
         <v>0</v>
       </c>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="11" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -3879,7 +3889,9 @@
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3">
+        <v>43736</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -3887,13 +3899,13 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -3902,7 +3914,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -3910,7 +3922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -3918,7 +3930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3332" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -3926,7 +3938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -3934,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -3942,7 +3954,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -3951,12 +3963,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add SaveHistory in SaveData frmTodoList
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -19,18 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Start at</t>
   </si>
   <si>
-    <t>10:35 AM</t>
+    <t>1:03 PM</t>
   </si>
   <si>
     <t>Lucky</t>
   </si>
   <si>
-    <t>True</t>
+    <t>False</t>
   </si>
   <si>
     <t xml:space="preserve">Today </t>
@@ -45,7 +45,7 @@
     <t>Incomplete</t>
   </si>
   <si>
-    <t>10/01/2019</t>
+    <t>10/02/2019</t>
   </si>
   <si>
     <t>History</t>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>09/27/2019</t>
+  </si>
+  <si>
+    <t>10/01/2019</t>
   </si>
   <si>
     <t>Achievement</t>
@@ -477,7 +480,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -3812,7 +3815,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -3820,7 +3823,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -3850,6 +3853,9 @@
       <c r="D8" s="2">
         <v>6</v>
       </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -3864,6 +3870,9 @@
       <c r="D9" s="2">
         <v>3</v>
       </c>
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -3878,6 +3887,9 @@
       <c r="D10" s="2">
         <v>3</v>
       </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -3892,7 +3904,9 @@
       <c r="D11" s="3">
         <v>43736</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -3901,30 +3915,30 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2">
         <v>3</v>
@@ -3932,7 +3946,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2">
         <v>4</v>
@@ -3940,7 +3954,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -3948,18 +3962,18 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Reset all frmDetail
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Start at</t>
   </si>
@@ -61,15 +61,6 @@
   </si>
   <si>
     <t>DateTime</t>
-  </si>
-  <si>
-    <t>09/26/2019</t>
-  </si>
-  <si>
-    <t>09/27/2019</t>
-  </si>
-  <si>
-    <t>10/01/2019</t>
   </si>
   <si>
     <t>Achievement</t>
@@ -437,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DXD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,8 +439,8 @@
     <col min="3" max="3" width="11.42578125" customWidth="1" style="2"/>
     <col min="4" max="8" bestFit="1" width="9.7109375" customWidth="1" style="2"/>
     <col min="9" max="10" bestFit="1" width="10.7109375" customWidth="1" style="2"/>
-    <col min="11" max="40" width="9.140625" customWidth="1" style="2"/>
-    <col min="41" max="16384" width="9.140625" customWidth="1" style="2"/>
+    <col min="11" max="45" width="9.140625" customWidth="1" style="2"/>
+    <col min="46" max="16384" width="9.140625" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3844,69 +3835,32 @@
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
-        <v>6</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2">
-        <v>3</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
+      <c r="H9" s="2"/>
+      <c r="M9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>3</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
+      <c r="D10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="3">
-        <v>43736</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -3915,46 +3869,46 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -3962,18 +3916,18 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add clear history targets when reset
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -24,7 +24,7 @@
     <t>Start at</t>
   </si>
   <si>
-    <t>1:03 PM</t>
+    <t>4:23 PM</t>
   </si>
   <si>
     <t>Lucky</t>
@@ -45,7 +45,7 @@
     <t>Incomplete</t>
   </si>
   <si>
-    <t>10/02/2019</t>
+    <t>10/05/2019</t>
   </si>
   <si>
     <t>History</t>
@@ -471,7 +471,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -3806,7 +3806,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -3814,7 +3814,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -3836,6 +3836,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -3843,6 +3844,8 @@
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
       <c r="H9" s="2"/>
       <c r="M9" s="2"/>
     </row>
@@ -3850,6 +3853,8 @@
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="K10" s="2"/>
     </row>

</xml_diff>

<commit_message>
SaveTodayTargets when change frm
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -471,7 +471,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -3806,7 +3806,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -3814,7 +3814,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Create Setup file, add some icon files
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -19,18 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Start at</t>
   </si>
   <si>
-    <t>4:23 PM</t>
-  </si>
-  <si>
     <t>Lucky</t>
-  </si>
-  <si>
-    <t>True</t>
   </si>
   <si>
     <t xml:space="preserve">Today </t>
@@ -428,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DXD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,36 +433,36 @@
     <col min="3" max="3" width="11.42578125" customWidth="1" style="2"/>
     <col min="4" max="8" bestFit="1" width="9.7109375" customWidth="1" style="2"/>
     <col min="9" max="10" bestFit="1" width="10.7109375" customWidth="1" style="2"/>
-    <col min="11" max="45" width="9.140625" customWidth="1" style="2"/>
-    <col min="46" max="16384" width="9.140625" customWidth="1" style="2"/>
+    <col min="11" max="47" width="9.140625" customWidth="1" style="2"/>
+    <col min="48" max="16384" width="9.140625" customWidth="1" style="2"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="5">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
+      <c r="D1" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="E1" s="2">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -3803,7 +3797,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -3811,7 +3805,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -3819,48 +3813,36 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="6"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="M9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="K10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -3874,13 +3856,13 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -3889,7 +3871,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -3897,7 +3879,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2">
         <v>0</v>
@@ -3905,7 +3887,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -3913,7 +3895,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -3921,7 +3903,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -3929,7 +3911,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Change some infomation about the product and complete version 1.0
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -19,12 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Start at</t>
   </si>
   <si>
-    <t>3:55 PM</t>
+    <t>7:30 AM</t>
   </si>
   <si>
     <t>Lucky</t>
@@ -45,7 +45,7 @@
     <t>Incomplete</t>
   </si>
   <si>
-    <t>10/06/2019</t>
+    <t>10/07/2019</t>
   </si>
   <si>
     <t>History</t>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>10/05/2019</t>
+  </si>
+  <si>
+    <t>10/06/2019</t>
   </si>
   <si>
     <t>Achievement</t>
@@ -3841,6 +3844,9 @@
       <c r="B8" s="2">
         <v>0</v>
       </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -3849,6 +3855,9 @@
       <c r="B9" s="2">
         <v>0</v>
       </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -3857,6 +3866,9 @@
       <c r="B10" s="2">
         <v>0</v>
       </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -3865,7 +3877,9 @@
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -3876,13 +3890,13 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -3891,7 +3905,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -3899,15 +3913,15 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -3915,7 +3929,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -3923,7 +3937,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -3931,7 +3945,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Hide notifyIcon when open form and exit frm if existed
</commit_message>
<xml_diff>
--- a/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
+++ b/WhatchaDoin/WhatchaDoin/bin/Debug/Details.xlsx
@@ -19,12 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Start at</t>
   </si>
   <si>
-    <t>7:30 AM</t>
+    <t>7:34 AM</t>
   </si>
   <si>
     <t>Lucky</t>
@@ -45,7 +45,7 @@
     <t>Incomplete</t>
   </si>
   <si>
-    <t>10/07/2019</t>
+    <t>10/29/2019</t>
   </si>
   <si>
     <t>History</t>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>10/06/2019</t>
+  </si>
+  <si>
+    <t>10/07/2019</t>
   </si>
   <si>
     <t>Achievement</t>
@@ -3847,6 +3850,9 @@
       <c r="C8" s="2">
         <v>0</v>
       </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -3858,6 +3864,9 @@
       <c r="C9" s="2">
         <v>0</v>
       </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -3869,6 +3878,9 @@
       <c r="C10" s="2">
         <v>0</v>
       </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -3880,7 +3892,9 @@
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -3890,13 +3904,13 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2">
         <v>0</v>
@@ -3905,7 +3919,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -3913,15 +3927,15 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2">
         <v>0</v>
@@ -3929,7 +3943,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
@@ -3937,7 +3951,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2">
         <v>0</v>
@@ -3945,7 +3959,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2">
         <v>0</v>

</xml_diff>